<commit_message>
Enhance SnapMap with critical fixes and preview improvements
Major fixes:
- Fix setUploadedFile undefined error in FieldMapping component
- Resolve API validation errors by updating frontend MatchMethod types
- Fix SFTP credentials API error by adding missing cryptography dependencies
- Update encryption utilities to use PBKDF2HMAC for compatibility

New features:
- Add empty column toggle in PreviewCSV (default: hide empty columns)
- Enhanced generated field functionality with intelligent field info
- Improved status badges for AUTO/MANUAL/GENERATED mappings
- Smart field naming and sample data generation

Technical improvements:
- Updated requirements.txt with cryptography and paramiko packages
- Fixed encryption import compatibility issues
- Reorganized project structure and cleaned up legacy files
- Enhanced type safety with proper MatchMethod definitions

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/docs/schemas/ef_csv_schema/ef_pay_grade_add_csv_schema.xlsx
+++ b/docs/schemas/ef_csv_schema/ef_pay_grade_add_csv_schema.xlsx
@@ -735,7 +735,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -806,12 +806,12 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>salaryAmount</t>
+          <t>joiningBonus</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>Column name is just a sample and can be changed. Refer to documentation.</t>
+          <t>Column name is just a sample and can be changed to match your intake form variable. For numeric variables, provide comma-separated values in format: min,max,target (e.g., '100,200,150' where min=100, max=200, target=150). Min and max values are required for numeric fields; target is optional.</t>
         </is>
       </c>
       <c r="C3" s="2" t="inlineStr">
@@ -830,26 +830,74 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
+          <t>bonusPayFrequency</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>Column name is just a sample and can be changed. Refer to documentation.</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>String</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>Optional</t>
+        </is>
+      </c>
+      <c r="E4" s="2" t="inlineStr"/>
+      <c r="F4" s="2" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>basePayFrequency</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>Column name is just a sample and can be changed. Refer to documentation.</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>String</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>Optional</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="inlineStr"/>
+      <c r="F5" s="2" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
           <t>currency</t>
         </is>
       </c>
-      <c r="B4" s="2" t="inlineStr">
+      <c r="B6" s="2" t="inlineStr">
         <is>
           <t>Column name is just a sample and can be changed. Refer to documentation.</t>
         </is>
       </c>
-      <c r="C4" s="2" t="inlineStr">
+      <c r="C6" s="2" t="inlineStr">
         <is>
           <t>String</t>
         </is>
       </c>
-      <c r="D4" s="2" t="inlineStr">
-        <is>
-          <t>Optional</t>
-        </is>
-      </c>
-      <c r="E4" s="2" t="inlineStr"/>
-      <c r="F4" s="2" t="inlineStr">
+      <c r="D6" s="2" t="inlineStr">
+        <is>
+          <t>Optional</t>
+        </is>
+      </c>
+      <c r="E6" s="2" t="inlineStr"/>
+      <c r="F6" s="2" t="inlineStr">
         <is>
           <t>USD
 EUR
@@ -862,6 +910,150 @@
 INR</t>
         </is>
       </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>salaryAmount</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>Column name is just a sample and can be changed to match your intake form variable. For numeric variables, provide comma-separated values in format: min,max,target (e.g., '100,200,150' where min=100, max=200, target=150). Min and max values are required for numeric fields; target is optional.</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>Numeric</t>
+        </is>
+      </c>
+      <c r="D7" s="2" t="inlineStr">
+        <is>
+          <t>Optional</t>
+        </is>
+      </c>
+      <c r="E7" s="2" t="inlineStr"/>
+      <c r="F7" s="2" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>variableBonus</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>Column name is just a sample and can be changed to match your intake form variable. For numeric variables, provide comma-separated values in format: min,max,target (e.g., '100,200,150' where min=100, max=200, target=150). Min and max values are required for numeric fields; target is optional.</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>Numeric</t>
+        </is>
+      </c>
+      <c r="D8" s="2" t="inlineStr">
+        <is>
+          <t>Optional</t>
+        </is>
+      </c>
+      <c r="E8" s="2" t="inlineStr"/>
+      <c r="F8" s="2" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>stockOptionsAmount</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>Column name is just a sample and can be changed to match your intake form variable. For numeric variables, provide comma-separated values in format: min,max,target (e.g., '100,200,150' where min=100, max=200, target=150). Min and max values are required for numeric fields; target is optional.</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="inlineStr">
+        <is>
+          <t>Numeric</t>
+        </is>
+      </c>
+      <c r="D9" s="2" t="inlineStr">
+        <is>
+          <t>Optional</t>
+        </is>
+      </c>
+      <c r="E9" s="2" t="inlineStr"/>
+      <c r="F9" s="2" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>relocationBonus</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>Column name is just a sample and can be changed to match your intake form variable. For numeric variables, provide comma-separated values in format: min,max,target (e.g., '100,200,150' where min=100, max=200, target=150). Min and max values are required for numeric fields; target is optional.</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="inlineStr">
+        <is>
+          <t>Numeric</t>
+        </is>
+      </c>
+      <c r="D10" s="2" t="inlineStr">
+        <is>
+          <t>Optional</t>
+        </is>
+      </c>
+      <c r="E10" s="2" t="inlineStr"/>
+      <c r="F10" s="2" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>totalCompensation</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>Column name is just a sample and can be changed to match your intake form variable. For numeric variables, provide comma-separated values in format: min,max,target (e.g., '100,200,150' where min=100, max=200, target=150). Min and max values are required for numeric fields; target is optional.</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="inlineStr">
+        <is>
+          <t>Numeric</t>
+        </is>
+      </c>
+      <c r="D11" s="2" t="inlineStr">
+        <is>
+          <t>Optional</t>
+        </is>
+      </c>
+      <c r="E11" s="2" t="inlineStr"/>
+      <c r="F11" s="2" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>countryCode</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="inlineStr">
+        <is>
+          <t>Column name is just a sample and can be changed. Refer to documentation.</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="inlineStr">
+        <is>
+          <t>String</t>
+        </is>
+      </c>
+      <c r="D12" s="2" t="inlineStr">
+        <is>
+          <t>Optional</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="inlineStr"/>
+      <c r="F12" s="2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>